<commit_message>
Need to be saved
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Courses_StronQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariia\RubymineProjects\lesson8\tests_rspec\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="123">
   <si>
     <t>Functionality</t>
   </si>
@@ -365,9 +365,6 @@
     <t>tc_02</t>
   </si>
   <si>
-    <t>User can register with the correct credentials</t>
-  </si>
-  <si>
     <t>User should be redirected to
 Contact Details tab.</t>
   </si>
@@ -376,6 +373,33 @@
   </si>
   <si>
     <t>User should be over 18 years old to apply</t>
+  </si>
+  <si>
+    <t>tc_03</t>
+  </si>
+  <si>
+    <t>Prerequisites:tc_01                         1. Fill all required fields with incorrect on this step"Getting Started". 2. Click on the Next button.</t>
+  </si>
+  <si>
+    <t>User can pass the Getting Started section with correct credentials.</t>
+  </si>
+  <si>
+    <t>User should not be redirected to
+Contact Details tab.</t>
+  </si>
+  <si>
+    <t>User is redirected to
+Sign Up page</t>
+  </si>
+  <si>
+    <t>User is redirected to
+Contact Details tab.</t>
+  </si>
+  <si>
+    <t>User is still on Getting Started tab. The alert message occurred.</t>
+  </si>
+  <si>
+    <t>User can not pass the Getting Started section with incorrect credentials(Email and retyped email are different).</t>
   </si>
 </sst>
 </file>
@@ -530,7 +554,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -607,6 +631,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1347,7 +1374,7 @@
   <dimension ref="A1:K226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,10 +1435,12 @@
       <c r="D2" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="27"/>
+      <c r="F2" s="26" t="s">
+        <v>119</v>
+      </c>
       <c r="G2" s="28"/>
       <c r="H2" s="29">
         <v>1</v>
@@ -1426,18 +1455,20 @@
         <v>111</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="26" t="s">
+        <v>120</v>
+      </c>
       <c r="G3" s="28"/>
       <c r="H3" s="29">
         <v>1</v>
@@ -1446,18 +1477,28 @@
         <v>110</v>
       </c>
       <c r="J3" s="40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>121</v>
+      </c>
       <c r="G4" s="28"/>
       <c r="H4" s="29">
         <v>1</v>

</xml_diff>